<commit_message>
Updated time/description in timesheet
</commit_message>
<xml_diff>
--- a/Documentation/Contributions/TimeReport_AspenBoler.xlsx
+++ b/Documentation/Contributions/TimeReport_AspenBoler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN3907\plant-partner\Documentation\Contributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3923A33-F307-4897-97AF-637CFF73C407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CAFE70-BA81-4F13-AE32-B4DEA45F2D39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>Name:</t>
   </si>
@@ -167,7 +167,10 @@
     <t>Began looking through project requirements and making adjustments to ensure issues were updated, naming conventions were followed</t>
   </si>
   <si>
-    <t>Tested Fernando's wifi contributions</t>
+    <t>Tested Fernando's wifi contributions, altered circuit, and uploaded finished circuit onto Github</t>
+  </si>
+  <si>
+    <t>Continued documenting stuff for prototype submission</t>
   </si>
 </sst>
 </file>
@@ -741,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="73" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -767,7 +770,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E199)</f>
-        <v>1.6131944444444448</v>
+        <v>1.6125000000000003</v>
       </c>
       <c r="F1" s="15"/>
     </row>
@@ -1327,25 +1330,35 @@
       <c r="C29" s="17">
         <v>0.59027777777777779</v>
       </c>
-      <c r="D29" s="17"/>
+      <c r="D29" s="17">
+        <v>0.62430555555555556</v>
+      </c>
       <c r="E29" s="10">
         <f t="shared" si="0"/>
-        <v>-0.59027777777777779</v>
+        <v>3.4027777777777768E-2</v>
       </c>
       <c r="F29" s="13" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="7"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="17"/>
+      <c r="A30" s="7">
+        <v>45975</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="17">
+        <v>0.625</v>
+      </c>
       <c r="D30" s="17"/>
       <c r="E30" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F30" s="13"/>
+        <v>-0.625</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>

</xml_diff>

<commit_message>
I'm taking a break brb
</commit_message>
<xml_diff>
--- a/Documentation/Contributions/TimeReport_AspenBoler.xlsx
+++ b/Documentation/Contributions/TimeReport_AspenBoler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN3907\plant-partner\Documentation\Contributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0F92CD-2BF6-43C5-BCA8-5FACF02C7E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF37199-4AA8-4865-909D-7C9B64DD44C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
   <si>
     <t>Name:</t>
   </si>
@@ -173,10 +173,10 @@
     <t>Continued documenting stuff for prototype submission, made circuit diagrams, editted some issues discussed what needed to be continued for submissables</t>
   </si>
   <si>
-    <t>Modify project display, began creating report document and presentation</t>
-  </si>
-  <si>
-    <t>Continuing report</t>
+    <t>Modify project display, began creating report document</t>
+  </si>
+  <si>
+    <t>Continuing report, modified readme</t>
   </si>
 </sst>
 </file>
@@ -750,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="73" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -776,7 +776,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E199)</f>
-        <v>1.9666666666666672</v>
+        <v>2.5291666666666672</v>
       </c>
       <c r="F1" s="15"/>
     </row>
@@ -1399,18 +1399,24 @@
       <c r="C32" s="17">
         <v>0.46250000000000002</v>
       </c>
-      <c r="D32" s="17"/>
+      <c r="D32" s="17">
+        <v>0.5625</v>
+      </c>
       <c r="E32" s="10">
         <f t="shared" si="0"/>
-        <v>-0.46250000000000002</v>
+        <v>9.9999999999999978E-2</v>
       </c>
       <c r="F32" s="13" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="7"/>
-      <c r="B33" s="8"/>
+      <c r="A33" s="7">
+        <v>45976</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
       <c r="E33" s="10">

</xml_diff>

<commit_message>
Extra plant data structure removed
</commit_message>
<xml_diff>
--- a/Documentation/Contributions/TimeReport_AspenBoler.xlsx
+++ b/Documentation/Contributions/TimeReport_AspenBoler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN3907\plant-partner\Documentation\Contributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAD7B79F-C3FA-4417-837D-70A8D1914476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564BF5B3-2DDD-42D3-B205-F7AA8132FD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="53">
   <si>
     <t>Name:</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>Clean Up</t>
+  </si>
+  <si>
+    <t>Experimented with ADC peripheral on DAD and reworked the peripheral  so it only needs to call an initialization function in main, reworked some aspects of main to avoid bad outputs/improve organization,  removed extra plant data structure, created blinky module</t>
   </si>
 </sst>
 </file>
@@ -765,7 +768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="73" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="73" workbookViewId="0">
       <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
@@ -1524,7 +1527,9 @@
         <f t="shared" si="0"/>
         <v>-0.59027777777777779</v>
       </c>
-      <c r="F37" s="13"/>
+      <c r="F37" s="13" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="7"/>

</xml_diff>

<commit_message>
Provided set up for switch and LED that'll increase predictability of behavior
</commit_message>
<xml_diff>
--- a/Documentation/Contributions/TimeReport_AspenBoler.xlsx
+++ b/Documentation/Contributions/TimeReport_AspenBoler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN4908\plant-partner\Documentation\Contributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97922CAE-FB1C-43D2-9268-45A5D53CB481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2B2E15-370E-4AC7-BCC2-0CD888FD3761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -206,7 +206,7 @@
     <t>Main Rework</t>
   </si>
   <si>
-    <t>Started modifying main to more closely match a routine based off of received signal from database</t>
+    <t>Started modifying main to more closely match a routine based off of received signal from database. Also made some tickets and cleaned up code to be more organized and efficient</t>
   </si>
 </sst>
 </file>
@@ -780,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C20" zoomScale="73" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="73" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -806,7 +806,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E199)</f>
-        <v>2.5791666666666671</v>
+        <v>3.4104166666666669</v>
       </c>
       <c r="F1" s="15"/>
     </row>
@@ -1568,7 +1568,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
-        <v>46048</v>
+        <v>46038</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>55</v>
@@ -1576,10 +1576,12 @@
       <c r="C39" s="17">
         <v>0.74930555555555556</v>
       </c>
-      <c r="D39" s="17"/>
+      <c r="D39" s="17">
+        <v>0.83125000000000004</v>
+      </c>
       <c r="E39" s="10">
         <f t="shared" si="0"/>
-        <v>-0.74930555555555556</v>
+        <v>8.1944444444444486E-2</v>
       </c>
       <c r="F39" s="13" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
Included check-in meeting time
</commit_message>
<xml_diff>
--- a/Documentation/Contributions/TimeReport_AspenBoler.xlsx
+++ b/Documentation/Contributions/TimeReport_AspenBoler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN4908\plant-partner\Documentation\Contributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9566FFE-2AA3-48CB-AD7C-DE1D9E13AD7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE68E16-6A5A-4C2F-A655-B33A302140FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
   <si>
     <t>Name:</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>Created pin diagram showing which pins were used for what; Integrated fertilizer pump addition to PWM and main and tested it out</t>
+  </si>
+  <si>
+    <t>Check-in 6: Met with group &amp; Tyler, discussed what's gotten done and what needs to get done for alpha build, showed bought materials and began observing what modifications would be needed to integrate electronics into plastic build</t>
   </si>
 </sst>
 </file>
@@ -777,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="73" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="73" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -803,7 +806,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E199)</f>
-        <v>3.4527777777777779</v>
+        <v>3.5006944444444446</v>
       </c>
       <c r="F1" s="15"/>
     </row>
@@ -1612,13 +1615,19 @@
       <c r="B41" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="17"/>
-      <c r="D41" s="17"/>
+      <c r="C41" s="17">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D41" s="17">
+        <v>0.49236111111111114</v>
+      </c>
       <c r="E41" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F41" s="13"/>
+        <v>4.7916666666666718E-2</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="7"/>

</xml_diff>

<commit_message>
Beginning small main tweak
</commit_message>
<xml_diff>
--- a/Documentation/Contributions/TimeReport_AspenBoler.xlsx
+++ b/Documentation/Contributions/TimeReport_AspenBoler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN4908\plant-partner\Documentation\Contributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE68E16-6A5A-4C2F-A655-B33A302140FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1E1196-12B3-4726-8982-F1D02ADF3C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
   <si>
     <t>Name:</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>Check-in 6: Met with group &amp; Tyler, discussed what's gotten done and what needs to get done for alpha build, showed bought materials and began observing what modifications would be needed to integrate electronics into plastic build</t>
+  </si>
+  <si>
+    <t>Realized I should go ahead and have main set up for potential of boolean to change depending on if auto-scheduling/care is on</t>
   </si>
 </sst>
 </file>
@@ -780,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="73" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="C28" zoomScale="73" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -806,7 +809,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E199)</f>
-        <v>3.5006944444444446</v>
+        <v>2.771527777777778</v>
       </c>
       <c r="F1" s="15"/>
     </row>
@@ -1630,15 +1633,23 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="7"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="17"/>
+      <c r="A42" s="7">
+        <v>46045</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="17">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="D42" s="17"/>
       <c r="E42" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F42" s="13"/>
+        <v>-0.72916666666666663</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="7"/>

</xml_diff>

<commit_message>
Added start time and def
</commit_message>
<xml_diff>
--- a/Documentation/Contributions/TimeReport_AspenBoler.xlsx
+++ b/Documentation/Contributions/TimeReport_AspenBoler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN4908\plant-partner\Documentation\Contributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49E9013C-3478-456A-B25A-F8246A997A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0907D2FE-F13F-4AF1-B854-1A028028568A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
   <si>
     <t>Name:</t>
   </si>
@@ -210,6 +210,9 @@
   </si>
   <si>
     <t>Realized I should go ahead and have main set up for potential of boolean to change depending on if auto-scheduling/care is on;  Created/modified tickets in project hub.</t>
+  </si>
+  <si>
+    <t>Integrated PR into main; solder and heat shrinked additional wires to extend motor wire length</t>
   </si>
 </sst>
 </file>
@@ -783,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="73" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="C27" zoomScale="73" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -809,7 +812,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E199)</f>
-        <v>3.5430555555555556</v>
+        <v>2.9597222222222221</v>
       </c>
       <c r="F1" s="15"/>
     </row>
@@ -1654,15 +1657,23 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="7"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="17"/>
+      <c r="A43" s="7">
+        <v>46048</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" s="17">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="D43" s="17"/>
       <c r="E43" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F43" s="13"/>
+        <v>-0.58333333333333337</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="7"/>

</xml_diff>

<commit_message>
Put in the correct ESP32 (DEVKIT-V1) into Schematic. Updated the IO pin connections for ESP. Added Power supply system to SChematic. Need to update optocoupler symbol and footprint. Then routing shall commence
</commit_message>
<xml_diff>
--- a/Documentation/Contributions/TimeReport_AspenBoler.xlsx
+++ b/Documentation/Contributions/TimeReport_AspenBoler.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN3907\plant-partner\Documentation\Contributions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN4908\plant-partner\Documentation\Contributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2463FD-A3AE-4CE5-8639-604B84BEA5E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0907D2FE-F13F-4AF1-B854-1A028028568A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
   <si>
     <t>Name:</t>
   </si>
@@ -189,6 +189,30 @@
   </si>
   <si>
     <t>Begin working on powerpoint</t>
+  </si>
+  <si>
+    <t>Experimented with ADC peripheral on DAD and reworked the peripheral  so it only needs to call an initialization function in main, reworked some aspects of main to avoid bad outputs/improve organization,  removed extra plant data structure, created heartbeat module</t>
+  </si>
+  <si>
+    <t>Changed personal directory name and it killed everything, took me an hour but it forced me to reinstall everything to get it working</t>
+  </si>
+  <si>
+    <t>Started modifying main to more closely match a routine based off of received signal from database. Also made some tickets and cleaned up code to be more organized and efficient</t>
+  </si>
+  <si>
+    <t>Alpha Build</t>
+  </si>
+  <si>
+    <t>Created pin diagram showing which pins were used for what; Integrated fertilizer pump addition to PWM and main and tested it out</t>
+  </si>
+  <si>
+    <t>Check-in 6: Met with group &amp; Tyler, discussed what's gotten done and what needs to get done for alpha build, showed bought materials and began observing what modifications would be needed to integrate electronics into plastic build</t>
+  </si>
+  <si>
+    <t>Realized I should go ahead and have main set up for potential of boolean to change depending on if auto-scheduling/care is on;  Created/modified tickets in project hub.</t>
+  </si>
+  <si>
+    <t>Integrated PR into main; solder and heat shrinked additional wires to extend motor wire length</t>
   </si>
 </sst>
 </file>
@@ -762,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C18" zoomScale="73" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="C27" zoomScale="73" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -788,7 +812,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E199)</f>
-        <v>3.0500000000000003</v>
+        <v>2.9597222222222221</v>
       </c>
       <c r="F1" s="15"/>
     </row>
@@ -1507,81 +1531,149 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
+      <c r="A37" s="7">
+        <v>46030</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="17">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="D37" s="17">
+        <v>0.79166666666666663</v>
+      </c>
       <c r="E37" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F37" s="13"/>
+        <v>0.20138888888888884</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="17"/>
-      <c r="D38" s="17"/>
+      <c r="A38" s="7">
+        <v>46038</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="17">
+        <v>0.67222222222222228</v>
+      </c>
+      <c r="D38" s="17">
+        <v>0.74930555555555556</v>
+      </c>
       <c r="E38" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F38" s="13"/>
+        <v>7.7083333333333282E-2</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17"/>
+      <c r="A39" s="7">
+        <v>46038</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="17">
+        <v>0.74930555555555556</v>
+      </c>
+      <c r="D39" s="17">
+        <v>0.83125000000000004</v>
+      </c>
       <c r="E39" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F39" s="13"/>
+        <v>8.1944444444444486E-2</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="7"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17"/>
+      <c r="A40" s="7">
+        <v>46043</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C40" s="17">
+        <v>0.54513888888888884</v>
+      </c>
+      <c r="D40" s="17">
+        <v>0.58750000000000002</v>
+      </c>
       <c r="E40" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F40" s="13"/>
+        <v>4.2361111111111183E-2</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="7"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="17"/>
+      <c r="A41" s="7">
+        <v>46045</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="17">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D41" s="17">
+        <v>0.49236111111111114</v>
+      </c>
       <c r="E41" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F41" s="13"/>
+        <v>4.7916666666666718E-2</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="7"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="17"/>
+      <c r="A42" s="7">
+        <v>46045</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="17">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D42" s="17">
+        <v>0.77152777777777781</v>
+      </c>
       <c r="E42" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F42" s="13"/>
+        <v>4.2361111111111183E-2</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="7"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="17"/>
+      <c r="A43" s="7">
+        <v>46048</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" s="17">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="D43" s="17"/>
       <c r="E43" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F43" s="13"/>
+        <v>-0.58333333333333337</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="7"/>

</xml_diff>

<commit_message>
Better integrate ip thing + wired fertilizer
</commit_message>
<xml_diff>
--- a/Documentation/Contributions/TimeReport_AspenBoler.xlsx
+++ b/Documentation/Contributions/TimeReport_AspenBoler.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN4908\plant-partner\Documentation\Contributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57B6D692-978E-4765-B05B-EFFB91DFF375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C707EB-F9CB-4F8C-89A0-1942CF44942F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
   <si>
     <t>Name:</t>
   </si>
@@ -222,6 +222,9 @@
   </si>
   <si>
     <t>Merged wire motor branch</t>
+  </si>
+  <si>
+    <t>Met up with group to test demo. Also received another 12v to 5v adapt, so began wire stripping and attaching fertilizer motor to a new relay; Utilized double-sided tape to rework our wire structure to make it more sound/easier to use and understand</t>
   </si>
 </sst>
 </file>
@@ -795,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="73" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="B32" zoomScale="73" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -821,7 +824,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E199)</f>
-        <v>3.7034722222222221</v>
+        <v>3.2590277777777779</v>
       </c>
       <c r="F1" s="15"/>
     </row>
@@ -1729,15 +1732,23 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="7"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="17"/>
+      <c r="A46" s="7">
+        <v>46058</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46" s="17">
+        <v>0.44444444444444442</v>
+      </c>
       <c r="D46" s="17"/>
       <c r="E46" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F46" s="13"/>
+        <v>-0.44444444444444442</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="7"/>

</xml_diff>

<commit_message>
Update Documentation before beginning more work
</commit_message>
<xml_diff>
--- a/Documentation/Contributions/TimeReport_AspenBoler.xlsx
+++ b/Documentation/Contributions/TimeReport_AspenBoler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN4908\plant-partner\Documentation\Contributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2531A9F7-B380-4909-B441-39A40B86E0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D48DD3F-306B-4BF4-9FDD-087E50A57A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="67">
   <si>
     <t>Name:</t>
   </si>
@@ -228,6 +228,15 @@
   </si>
   <si>
     <t>Check-in 7: Met with group &amp; Tyler to demo alpha build; Discussed what needed to be done and experimented with group to get MQTT client to send a signal to the microcontroller.</t>
+  </si>
+  <si>
+    <t>Beta Build</t>
+  </si>
+  <si>
+    <t>Experimented with group and successfully got MQTT client to communicate t microcontroller. Started modifying main so the main loop would be triggered from MQTT message</t>
+  </si>
+  <si>
+    <t>Began cleaning up MQTT branch to prepare it for more clean merge</t>
   </si>
 </sst>
 </file>
@@ -801,8 +810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="73" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="C34" zoomScale="73" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -827,7 +836,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E199)</f>
-        <v>3.911111111111111</v>
+        <v>3.2298611111111111</v>
       </c>
       <c r="F1" s="15"/>
     </row>
@@ -1777,26 +1786,44 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="7"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="17"/>
+      <c r="A48" s="7">
+        <v>46063</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" s="17">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D48" s="17">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="E48" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F48" s="13"/>
+        <v>0.13888888888888895</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="7"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="17"/>
+      <c r="A49" s="7">
+        <v>46063</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" s="17">
+        <v>0.82013888888888886</v>
+      </c>
       <c r="D49" s="17"/>
       <c r="E49" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F49" s="13"/>
+        <v>-0.82013888888888886</v>
+      </c>
+      <c r="F49" s="13" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="7"/>

</xml_diff>

<commit_message>
Put in end time
</commit_message>
<xml_diff>
--- a/Documentation/Contributions/TimeReport_AspenBoler.xlsx
+++ b/Documentation/Contributions/TimeReport_AspenBoler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN4908\plant-partner\Documentation\Contributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FB4C2E-7DE1-4218-BB6B-DDD378AC328D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A48CBA8-4C56-4BF1-A8DE-27D85E08C9E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -251,7 +251,7 @@
     <t>Check-in 8: Met with group &amp; Tyler to demo current status of beta build;</t>
   </si>
   <si>
-    <t>Tested MQTT on my own computer to see it still works, merged into main, updated tickets, began working on finishing up what's left to integrate soil sensor</t>
+    <t>Tested MQTT on my own computer to see it still works, merged into main, updated tickets, set up rest of the code needed to test NPK sensor in person</t>
   </si>
 </sst>
 </file>
@@ -825,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C42" zoomScale="73" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="B44" zoomScale="73" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -851,7 +851,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E199)</f>
-        <v>2.7284722222222229</v>
+        <v>3.2993055555555557</v>
       </c>
       <c r="F1" s="15"/>
     </row>
@@ -1894,10 +1894,12 @@
       <c r="C52" s="17">
         <v>0.47291666666666665</v>
       </c>
-      <c r="D52" s="17"/>
+      <c r="D52" s="17">
+        <v>0.5708333333333333</v>
+      </c>
       <c r="E52" s="10">
         <f t="shared" si="0"/>
-        <v>-0.47291666666666665</v>
+        <v>9.7916666666666652E-2</v>
       </c>
       <c r="F52" s="13" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Check for today, changed led pin
</commit_message>
<xml_diff>
--- a/Documentation/Contributions/TimeReport_AspenBoler.xlsx
+++ b/Documentation/Contributions/TimeReport_AspenBoler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19042\Downloads\HW\CEN4908\plant-partner\Documentation\Contributions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEA1F46-C3CA-44D6-AA1A-9C6B6B17E06E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB323393-75F0-414C-9725-EA9BCBBCBEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{605B5A91-C2DF-4ED5-9E2C-366EB894E8F1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="79">
   <si>
     <t>Name:</t>
   </si>
@@ -267,6 +267,12 @@
   </si>
   <si>
     <t>Started testing NPK AND IT STILL DOESN'T WORK OH MY GOD</t>
+  </si>
+  <si>
+    <t>Got together as a goup and began planning phsyical layout of board</t>
+  </si>
+  <si>
+    <t>Finishing planning out board and began soldering. Got and tested LED and photoresistor</t>
   </si>
 </sst>
 </file>
@@ -840,8 +846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25321167-01B1-413D-AB29-4165F3CF20BA}">
   <dimension ref="A1:F199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="73" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="B58" zoomScale="73" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -866,7 +872,7 @@
       </c>
       <c r="E1" s="6">
         <f>SUM(E4:E199)</f>
-        <v>4.7048611111111107</v>
+        <v>4.9604166666666663</v>
       </c>
       <c r="F1" s="15"/>
     </row>
@@ -2068,26 +2074,42 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="7"/>
-      <c r="B60" s="8"/>
-      <c r="C60" s="17"/>
-      <c r="D60" s="17"/>
+      <c r="A60" s="7">
+        <v>46070</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C60" s="17">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="D60" s="17">
+        <v>0.53333333333333333</v>
+      </c>
       <c r="E60" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F60" s="13"/>
+        <v>8.8888888888888906E-2</v>
+      </c>
+      <c r="F60" s="13" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="7"/>
       <c r="B61" s="8"/>
-      <c r="C61" s="17"/>
-      <c r="D61" s="17"/>
+      <c r="C61" s="17">
+        <v>0.57430555555555551</v>
+      </c>
+      <c r="D61" s="17">
+        <v>0.74097222222222225</v>
+      </c>
       <c r="E61" s="10">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F61" s="13"/>
+        <v>0.16666666666666674</v>
+      </c>
+      <c r="F61" s="13" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="7"/>

</xml_diff>